<commit_message>
Update to user data
</commit_message>
<xml_diff>
--- a/user-data/2013-p20-population/2013-p20-population.xlsx
+++ b/user-data/2013-p20-population/2013-p20-population.xlsx
@@ -1051,13 +1051,13 @@
     <t xml:space="preserve">Name: 2013-p20-population</t>
   </si>
   <si>
-    <t xml:space="preserve">Description: The approximate number of people in each country who are in the global poorest 20%</t>
+    <t xml:space="preserve">Description: The approximate number of people in each country who are in the global poorest 20%. . 2013 represents the most recent year data is available.</t>
   </si>
   <si>
     <t xml:space="preserve">Units of measure: unit</t>
   </si>
   <si>
-    <t xml:space="preserve">Source: 58</t>
+    <t xml:space="preserve">Source: 59</t>
   </si>
   <si>
     <t xml:space="preserve">Source-link: 1</t>

</xml_diff>

<commit_message>
New user data, including pneumonia
</commit_message>
<xml_diff>
--- a/user-data/2013-p20-population/2013-p20-population.xlsx
+++ b/user-data/2013-p20-population/2013-p20-population.xlsx
@@ -1051,13 +1051,13 @@
     <t xml:space="preserve">Name: 2013-p20-population</t>
   </si>
   <si>
-    <t xml:space="preserve">Description: The approximate number of people in each country who are in the global poorest 20%</t>
+    <t xml:space="preserve">Description: The approximate number of people in each country who are in the global poorest 20%. . 2013 represents the most recent year data is available.</t>
   </si>
   <si>
     <t xml:space="preserve">Units of measure: unit</t>
   </si>
   <si>
-    <t xml:space="preserve">Source: 58</t>
+    <t xml:space="preserve">Source: 60</t>
   </si>
   <si>
     <t xml:space="preserve">Source-link: 1</t>

</xml_diff>